<commit_message>
Added full planning tests for the first sprint
</commit_message>
<xml_diff>
--- a/Documentation/Tests/Artificial Intelligence/Test_Planning_Prolog_Sprint1.xlsx
+++ b/Documentation/Tests/Artificial Intelligence/Test_Planning_Prolog_Sprint1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago\Documents\LAPR5\Documentation\Tests\Artificial Intelligence\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
   <si>
     <t>Area</t>
   </si>
@@ -90,6 +90,24 @@
   </si>
   <si>
     <t>false</t>
+  </si>
+  <si>
+    <t>breadth_search('JoseCid','Joao',L)</t>
+  </si>
+  <si>
+    <t>isFriend('Tiago','Tiago').</t>
+  </si>
+  <si>
+    <t>False</t>
+  </si>
+  <si>
+    <t>L=['Joao','Diogo','Francisco','JoseCid']</t>
+  </si>
+  <si>
+    <t>breadth_search('Artur',Stephanie',L)</t>
+  </si>
+  <si>
+    <t>L=['Artur','Tiago','Stephanie']</t>
   </si>
 </sst>
 </file>
@@ -498,16 +516,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B9:E30"/>
+  <dimension ref="B9:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="3" width="32" customWidth="1"/>
+    <col min="3" max="3" width="34.5703125" customWidth="1"/>
     <col min="4" max="4" width="75.5703125" customWidth="1"/>
     <col min="5" max="5" width="78.140625" customWidth="1"/>
   </cols>
@@ -606,8 +624,53 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C30" s="3"/>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C32" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
More tests of our predicates added to the file of the tests
</commit_message>
<xml_diff>
--- a/Documentation/Tests/Artificial Intelligence/Test_Planning_Prolog_Sprint1.xlsx
+++ b/Documentation/Tests/Artificial Intelligence/Test_Planning_Prolog_Sprint1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="34">
   <si>
     <t>Area</t>
   </si>
@@ -108,6 +108,24 @@
   </si>
   <si>
     <t>L=['Artur','Tiago','Stephanie']</t>
+  </si>
+  <si>
+    <t>branch_and_bound('Vicky','JoseCid',L)</t>
+  </si>
+  <si>
+    <t>L=['Vicky','Joao','Tiago','Diogo','Francisco','JoseCid']</t>
+  </si>
+  <si>
+    <t>branch_and_bound('Simao','Maria',L)</t>
+  </si>
+  <si>
+    <t>L=[Simao','Artur','Tiago','Stephanie','Maria']</t>
+  </si>
+  <si>
+    <t>Note: Some bugs of branch_and_bound need to be fixed</t>
+  </si>
+  <si>
+    <t>branch_and_bound('Joao','Tiago',L)</t>
   </si>
 </sst>
 </file>
@@ -518,8 +536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B9:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -666,7 +684,52 @@
         <v>27</v>
       </c>
     </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" t="s">
+        <v>31</v>
+      </c>
+      <c r="E21" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>32</v>
+      </c>
       <c r="C30" s="3"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added list of testes of search predicates
</commit_message>
<xml_diff>
--- a/Documentation/Tests/Artificial Intelligence/Test_Planning_Prolog_Sprint1.xlsx
+++ b/Documentation/Tests/Artificial Intelligence/Test_Planning_Prolog_Sprint1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
   <si>
     <t>Area</t>
   </si>
@@ -110,12 +110,6 @@
     <t>L=['Artur','Tiago','Stephanie']</t>
   </si>
   <si>
-    <t>branch_and_bound('Vicky','JoseCid',L)</t>
-  </si>
-  <si>
-    <t>L=['Vicky','Joao','Tiago','Diogo','Francisco','JoseCid']</t>
-  </si>
-  <si>
     <t>branch_and_bound('Simao','Maria',L)</t>
   </si>
   <si>
@@ -126,6 +120,45 @@
   </si>
   <si>
     <t>branch_and_bound('Joao','Tiago',L)</t>
+  </si>
+  <si>
+    <t>branch_and_bound('Joao','JoseCid',L)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L=[' Joao','Tiago','Stephanie','Diogo','Francisco','JoseCid']                                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">L=[' Joao','Tiago','Stephanie','Diogo','Francisco','JoseCid']    </t>
+  </si>
+  <si>
+    <t>L=[Simao','Joao','Tiago','Stephanie','Maria']</t>
+  </si>
+  <si>
+    <t>L=['Joao','Tiago']</t>
+  </si>
+  <si>
+    <t>branch_and_bound('Tiago','Joao',L)</t>
+  </si>
+  <si>
+    <t>L=['Tiago','Joao']</t>
+  </si>
+  <si>
+    <t>branch_and_bound('Andre','Nando')</t>
+  </si>
+  <si>
+    <t>L=['Andre','Tiago','Stephanie','Diogo','Joao','Simao','Artur','Alcides','Nando']</t>
+  </si>
+  <si>
+    <t>L=['Tiago','Stephanie','Diogo','Joao']</t>
+  </si>
+  <si>
+    <t>branch_and_bound('JoseCid','Maria')</t>
+  </si>
+  <si>
+    <t>L=['JoseCid','Francisco','Diogo','Stephanie','Maria']</t>
+  </si>
+  <si>
+    <t>L=['JoseCid','Francisco','Diogo','Tiago','Stephanie','Maria']</t>
   </si>
 </sst>
 </file>
@@ -536,14 +569,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B9:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="3" width="34.5703125" customWidth="1"/>
+    <col min="3" max="3" width="47.5703125" customWidth="1"/>
     <col min="4" max="4" width="75.5703125" customWidth="1"/>
     <col min="5" max="5" width="78.140625" customWidth="1"/>
   </cols>
@@ -689,13 +722,13 @@
         <v>14</v>
       </c>
       <c r="C20" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E20" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
@@ -703,13 +736,13 @@
         <v>14</v>
       </c>
       <c r="C21" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D21" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E21" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
@@ -717,18 +750,60 @@
         <v>14</v>
       </c>
       <c r="C22" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D22" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>16</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" t="s">
+        <v>40</v>
+      </c>
+      <c r="E24" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C30" s="3"/>
     </row>

</xml_diff>